<commit_message>
updated events so only future events show
</commit_message>
<xml_diff>
--- a/Resources/events_for_website.xlsx
+++ b/Resources/events_for_website.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elbor\Box\ADSC\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6354756B-75EF-463F-A396-DE9016035DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168C240C-D8B6-47DF-BF3A-28EB5CA2878E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="3110" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -63,10 +63,52 @@
     <t>10:00 AM</t>
   </si>
   <si>
-    <t>Thursday, 1 June 2023</t>
-  </si>
-  <si>
-    <t>Thursday, 29 June 2023</t>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>1 June 2023</t>
+  </si>
+  <si>
+    <t>29 June 2023</t>
+  </si>
+  <si>
+    <t>9 March 2023</t>
+  </si>
+  <si>
+    <t>Dino Sejdinovic</t>
+  </si>
+  <si>
+    <t>Jack Valmadre</t>
+  </si>
+  <si>
+    <t>Hierarchical Classification</t>
+  </si>
+  <si>
+    <t>27 April 2023</t>
+  </si>
+  <si>
+    <t>15 May 2023</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tobin South</t>
+  </si>
+  <si>
+    <t>SANTOS Petroleum Engineering G04</t>
+  </si>
+  <si>
+    <t>12:00 PM</t>
+  </si>
+  <si>
+    <t>"ChatGPT is the future of data science" &amp; other things people at MIT can't stop staying</t>
+  </si>
+  <si>
+    <t>The rise of ChatGPT as a tool for writing data science code follows a long history of tools aims at democratizing data science.  While not the end of coding or data science, it does present a new paradigm of how users can interact with information systems in flexible ways. This talk, featuring a guest project showcase from Peter Moskvichev, will examine how the way organizations, communities, and individuals interact with their data, from LLM data science interfaces, secure community data pools, novel privacy preservation tools, and zero-knowledge proofs. It will feature work from around the MIT Media Lab and will foster some discussion about how translational research can be kicked into overdrive.</t>
   </si>
 </sst>
 </file>
@@ -102,10 +144,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,77 +436,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.90625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" customWidth="1"/>
-    <col min="4" max="4" width="12" style="2" customWidth="1"/>
-    <col min="5" max="5" width="32.6328125" customWidth="1"/>
+    <col min="1" max="2" width="21.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.6328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="79.6328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>